<commit_message>
Setup student screen in multiple logins
</commit_message>
<xml_diff>
--- a/public/excel/StudentData.xlsx
+++ b/public/excel/StudentData.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vaishnav\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE87E333-63E3-47ED-9E98-09BB14A15934}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="52">
   <si>
     <t>First Name</t>
   </si>
@@ -164,33 +173,37 @@
   </si>
   <si>
     <t>india11</t>
+  </si>
+  <si>
+    <t>Pending</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -201,7 +214,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -211,38 +224,42 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -432,29 +449,34 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="10.5"/>
-    <col customWidth="1" min="2" max="2" width="10.13"/>
-    <col customWidth="1" min="3" max="3" width="16.13"/>
-    <col customWidth="1" min="4" max="4" width="13.63"/>
-    <col customWidth="1" min="5" max="5" width="19.5"/>
-    <col customWidth="1" min="6" max="6" width="17.0"/>
-    <col customWidth="1" min="7" max="7" width="20.75"/>
+    <col min="1" max="1" width="10.453125" customWidth="1"/>
+    <col min="2" max="2" width="10.08984375" customWidth="1"/>
+    <col min="3" max="3" width="16.08984375" customWidth="1"/>
+    <col min="4" max="4" width="13.6328125" customWidth="1"/>
+    <col min="5" max="5" width="19.453125" customWidth="1"/>
+    <col min="6" max="6" width="17" customWidth="1"/>
+    <col min="7" max="7" width="20.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -477,7 +499,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -488,13 +510,19 @@
         <v>9</v>
       </c>
       <c r="D2" s="3">
-        <v>1.23213213E8</v>
+        <v>123213213</v>
+      </c>
+      <c r="E2" s="4">
+        <v>45265</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3">
+      <c r="G2" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
@@ -505,13 +533,19 @@
         <v>13</v>
       </c>
       <c r="D3" s="3">
-        <v>1.23213214E8</v>
+        <v>123213214</v>
+      </c>
+      <c r="E3" s="4">
+        <v>45266</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4">
+      <c r="G3" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>15</v>
       </c>
@@ -522,13 +556,19 @@
         <v>17</v>
       </c>
       <c r="D4" s="3">
-        <v>1.23213215E8</v>
+        <v>123213215</v>
+      </c>
+      <c r="E4" s="4">
+        <v>45267</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5">
+      <c r="G4" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>19</v>
       </c>
@@ -539,13 +579,19 @@
         <v>21</v>
       </c>
       <c r="D5" s="3">
-        <v>1.23213216E8</v>
+        <v>123213216</v>
+      </c>
+      <c r="E5" s="4">
+        <v>45268</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6">
+      <c r="G5" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>23</v>
       </c>
@@ -556,13 +602,19 @@
         <v>25</v>
       </c>
       <c r="D6" s="3">
-        <v>1.23213217E8</v>
+        <v>123213217</v>
+      </c>
+      <c r="E6" s="4">
+        <v>45269</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="7">
+      <c r="G6" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>27</v>
       </c>
@@ -573,13 +625,19 @@
         <v>29</v>
       </c>
       <c r="D7" s="3">
-        <v>1.23213218E8</v>
+        <v>123213218</v>
+      </c>
+      <c r="E7" s="4">
+        <v>45270</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="8">
+      <c r="G7" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>31</v>
       </c>
@@ -590,13 +648,19 @@
         <v>33</v>
       </c>
       <c r="D8" s="3">
-        <v>1.23213219E8</v>
+        <v>123213219</v>
+      </c>
+      <c r="E8" s="4">
+        <v>45271</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="9">
+      <c r="G8" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>35</v>
       </c>
@@ -607,13 +671,19 @@
         <v>37</v>
       </c>
       <c r="D9" s="3">
-        <v>1.2321322E8</v>
+        <v>123213220</v>
+      </c>
+      <c r="E9" s="4">
+        <v>45272</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="10">
+      <c r="G9" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>39</v>
       </c>
@@ -624,13 +694,19 @@
         <v>41</v>
       </c>
       <c r="D10" s="3">
-        <v>1.23213221E8</v>
+        <v>123213221</v>
+      </c>
+      <c r="E10" s="4">
+        <v>45273</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="11">
+      <c r="G10" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>43</v>
       </c>
@@ -641,13 +717,19 @@
         <v>45</v>
       </c>
       <c r="D11" s="3">
-        <v>1.23213222E8</v>
+        <v>123213222</v>
+      </c>
+      <c r="E11" s="4">
+        <v>45274</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="12">
+      <c r="G11" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>47</v>
       </c>
@@ -658,13 +740,20 @@
         <v>49</v>
       </c>
       <c r="D12" s="3">
-        <v>1.23213223E8</v>
+        <v>123213223</v>
+      </c>
+      <c r="E12" s="4">
+        <v>45275</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>50</v>
       </c>
+      <c r="G12" s="3" t="s">
+        <v>51</v>
+      </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Assign and bulk assign consultant staff api integration
</commit_message>
<xml_diff>
--- a/public/excel/StudentData.xlsx
+++ b/public/excel/StudentData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vaishnav\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE87E333-63E3-47ED-9E98-09BB14A15934}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D54FD5C-465B-445F-A1CA-57DCD0C1DAF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="53">
   <si>
     <t>First Name</t>
   </si>
@@ -176,6 +176,9 @@
   </si>
   <si>
     <t>Pending</t>
+  </si>
+  <si>
+    <t>SOURCE</t>
   </si>
 </sst>
 </file>
@@ -459,24 +462,24 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.453125" customWidth="1"/>
-    <col min="2" max="2" width="10.08984375" customWidth="1"/>
+    <col min="1" max="1" width="14.1796875" customWidth="1"/>
+    <col min="2" max="2" width="13.08984375" customWidth="1"/>
     <col min="3" max="3" width="16.08984375" customWidth="1"/>
     <col min="4" max="4" width="13.6328125" customWidth="1"/>
     <col min="5" max="5" width="19.453125" customWidth="1"/>
-    <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="20.7265625" customWidth="1"/>
+    <col min="6" max="6" width="23" customWidth="1"/>
+    <col min="7" max="7" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -498,8 +501,11 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H1" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -521,8 +527,11 @@
       <c r="G2" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
@@ -544,8 +553,11 @@
       <c r="G3" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>15</v>
       </c>
@@ -567,8 +579,11 @@
       <c r="G4" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>19</v>
       </c>
@@ -590,8 +605,11 @@
       <c r="G5" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>23</v>
       </c>
@@ -613,8 +631,11 @@
       <c r="G6" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>27</v>
       </c>
@@ -636,8 +657,11 @@
       <c r="G7" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>31</v>
       </c>
@@ -659,8 +683,11 @@
       <c r="G8" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>35</v>
       </c>
@@ -682,8 +709,11 @@
       <c r="G9" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>39</v>
       </c>
@@ -705,8 +735,11 @@
       <c r="G10" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>43</v>
       </c>
@@ -728,8 +761,11 @@
       <c r="G11" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="H11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>47</v>
       </c>
@@ -750,6 +786,9 @@
       </c>
       <c r="G12" s="3" t="s">
         <v>51</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>